<commit_message>
Fixed Electrolysis Excel file
</commit_message>
<xml_diff>
--- a/DWSIM/Assets/samples/Electrolysis.xlsx
+++ b/DWSIM/Assets/samples/Electrolysis.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\Visual Studio 2013\Projects\DWSIM3\DWSIM\bin\Release\samples\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="14115" windowHeight="4170" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="14115" windowHeight="4170" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
     <sheet name="Output" sheetId="2" r:id="rId2"/>
     <sheet name="Calculations" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -679,6 +684,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -726,7 +734,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -761,7 +769,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -974,7 +982,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1124,10 +1132,10 @@
     </row>
     <row r="12" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B12" s="4">
-        <v>15.419249390939701</v>
+        <v>0</v>
       </c>
       <c r="H12" s="8"/>
     </row>
@@ -1142,10 +1150,10 @@
     </row>
     <row r="14" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B14" s="4">
-        <v>0</v>
+        <v>15.419249390939662</v>
       </c>
       <c r="H14" s="8"/>
     </row>
@@ -1183,8 +1191,8 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1350,11 +1358,11 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B12">
-        <f>Input!B12+Calculations!B15</f>
-        <v>15.367428045009069</v>
+        <f>Input!B12+Calculations!B16</f>
+        <v>5.1821345930632687E-2</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -1368,11 +1376,11 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B14">
-        <f>Input!B14+Calculations!B16</f>
-        <v>5.1821345930632687E-2</v>
+        <f>Input!B14+Calculations!B15</f>
+        <v>15.36742804500903</v>
       </c>
     </row>
   </sheetData>
@@ -1385,8 +1393,8 @@
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1595,8 +1603,8 @@
         <v>32</v>
       </c>
       <c r="B26" s="1">
-        <f>Input!B12*B25/1000</f>
-        <v>0.27754648903691465</v>
+        <f>Input!B14*B25/1000</f>
+        <v>0.27754648903691392</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>53</v>
@@ -1608,7 +1616,7 @@
       </c>
       <c r="B27" s="1">
         <f>B23/B24/B26</f>
-        <v>4.9014558472553533</v>
+        <v>4.9014558472553658</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Update Electrolysis Excel sample file
</commit_message>
<xml_diff>
--- a/DWSIM/Assets/samples/Electrolysis.xlsx
+++ b/DWSIM/Assets/samples/Electrolysis.xlsx
@@ -1,27 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\Visual Studio 2013\Projects\DWSIM3\DWSIM\bin\Release\samples\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="14115" windowHeight="4170" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="14115" windowHeight="4170" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
     <sheet name="Output" sheetId="2" r:id="rId2"/>
     <sheet name="Calculations" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="63">
   <si>
     <t>Input streams to Unit</t>
   </si>
@@ -107,12 +102,6 @@
     <t>Voltage of single cell in stack</t>
   </si>
   <si>
-    <t>ElectricalpPower consumption of electrolysis</t>
-  </si>
-  <si>
-    <t>Electrical current to electrolysis cells</t>
-  </si>
-  <si>
     <t>Total voltage of cell stack</t>
   </si>
   <si>
@@ -147,6 +136,63 @@
   </si>
   <si>
     <t>Reaction:</t>
+  </si>
+  <si>
+    <t>Reaction Extend:</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>O2</t>
+  </si>
+  <si>
+    <t>Model of water electrolysis</t>
+  </si>
+  <si>
+    <t>Standard Potential O2</t>
+  </si>
+  <si>
+    <t>Waste Heat</t>
+  </si>
+  <si>
+    <t>Calculation of waste heat</t>
+  </si>
+  <si>
+    <t>Heat capacity water</t>
+  </si>
+  <si>
+    <t>KJ/Kg/K</t>
+  </si>
+  <si>
+    <t>MW water</t>
+  </si>
+  <si>
+    <t>Kg/s</t>
+  </si>
+  <si>
+    <t>dT</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Power utilisiation efficiency</t>
+  </si>
+  <si>
+    <t>Yield</t>
+  </si>
+  <si>
+    <t>Exit</t>
+  </si>
+  <si>
+    <t>g/mol</t>
+  </si>
+  <si>
+    <t>Electrical Power consumption of electrolysis</t>
   </si>
   <si>
     <r>
@@ -169,7 +215,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>O + 4e</t>
+      <t>O -&gt; (4e</t>
     </r>
     <r>
       <rPr>
@@ -188,7 +234,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> -&gt; 2 H</t>
+      <t xml:space="preserve"> ) -&gt; 2 H</t>
     </r>
     <r>
       <rPr>
@@ -221,58 +267,13 @@
     </r>
   </si>
   <si>
-    <t>Reaction Extend:</t>
-  </si>
-  <si>
-    <t>H2</t>
-  </si>
-  <si>
-    <t>O2</t>
-  </si>
-  <si>
-    <t>Model of water electrolysis</t>
-  </si>
-  <si>
-    <t>Standard Potential O2</t>
-  </si>
-  <si>
-    <t>Waste Heat</t>
-  </si>
-  <si>
-    <t>Calculation of waste heat</t>
-  </si>
-  <si>
-    <t>Heat capacity water</t>
-  </si>
-  <si>
-    <t>KJ/Kg/K</t>
-  </si>
-  <si>
-    <t>MW water</t>
-  </si>
-  <si>
-    <t>Kg/s</t>
-  </si>
-  <si>
-    <t>dT</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
-    <t>Power utilisiation efficiency</t>
-  </si>
-  <si>
-    <t>Yield</t>
-  </si>
-  <si>
-    <t>Exit</t>
-  </si>
-  <si>
-    <t>g/mol</t>
+    <t>Water massflow</t>
+  </si>
+  <si>
+    <t>Overvoltage</t>
+  </si>
+  <si>
+    <t>Electrical current of electrolysis cells</t>
   </si>
 </sst>
 </file>
@@ -676,7 +677,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -692,9 +693,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -732,9 +733,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -769,7 +770,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -804,7 +805,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -982,10 +983,10 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" style="6"/>
@@ -1036,7 +1037,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -1051,7 +1052,7 @@
         <v>19</v>
       </c>
       <c r="J5" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -1074,7 +1075,7 @@
         <v>23</v>
       </c>
       <c r="J6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -1097,7 +1098,7 @@
         <v>22</v>
       </c>
       <c r="J7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -1132,7 +1133,7 @@
     </row>
     <row r="12" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B12" s="4">
         <v>0</v>
@@ -1141,7 +1142,7 @@
     </row>
     <row r="13" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B13" s="4">
         <v>0</v>
@@ -1150,7 +1151,7 @@
     </row>
     <row r="14" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14" s="4">
         <v>15.419249390939662</v>
@@ -1191,14 +1192,14 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="10" max="10" width="33.7109375" customWidth="1"/>
+    <col min="10" max="10" width="38.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" x14ac:dyDescent="0.3">
@@ -1245,7 +1246,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -1261,7 +1262,7 @@
         <v>25</v>
       </c>
       <c r="J5" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -1319,17 +1320,17 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H7">
         <f>Calculations!B20/Output!H6*100</f>
         <v>68.333333333333329</v>
       </c>
       <c r="I7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="J7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -1358,7 +1359,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B12">
         <f>Input!B12+Calculations!B16</f>
@@ -1367,7 +1368,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B13">
         <f>Input!B13+Calculations!B17</f>
@@ -1376,7 +1377,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14">
         <f>Input!B14+Calculations!B15</f>
@@ -1393,25 +1394,26 @@
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="34" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B2" s="34"/>
       <c r="C2" s="34"/>
@@ -1419,13 +1421,13 @@
     <row r="4" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B5" s="25">
         <v>96485.336500000005</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -1443,7 +1445,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B8" s="1">
         <f>Input!H7</f>
@@ -1453,23 +1455,23 @@
     </row>
     <row r="9" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B9" s="22">
         <f>B7/B5*B8</f>
         <v>0.10364269186126537</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="C12" s="12"/>
     </row>
@@ -1480,58 +1482,58 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="29" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B14" s="30"/>
       <c r="C14" s="31"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="32" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" s="1">
         <f>-B9/4*2</f>
         <v>-5.1821345930632687E-2</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="32" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B16" s="1">
         <f>B9/4*2</f>
         <v>5.1821345930632687E-2</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B17" s="22">
         <f>B9/4*1</f>
         <v>2.5910672965316343E-2</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="12"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B20" s="1">
         <v>1.23</v>
@@ -1554,7 +1556,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B22" s="1">
         <f>B21-B20</f>
@@ -1566,7 +1568,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B23" s="1">
         <f>B22*B7*B8/1000</f>
@@ -1578,48 +1580,48 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B24" s="1">
         <v>4.1900000000000004</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B25" s="1">
         <v>18</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="B26" s="1">
         <f>Input!B14*B25/1000</f>
         <v>0.27754648903691392</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B27" s="1">
         <f>B23/B24/B26</f>
         <v>4.9014558472553658</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>